<commit_message>
More secure calling structure.
</commit_message>
<xml_diff>
--- a/doc/moodle_api_functions.xlsx
+++ b/doc/moodle_api_functions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glah/Documents/code/github/moodle-autopilot/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316EA278-FC38-D14A-9223-1498AE3D4144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843202FE-C9EE-9546-BBDA-84B812BE6ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62400" yWindow="-10300" windowWidth="22360" windowHeight="28300" xr2:uid="{FA1526C8-0ACF-E742-8A11-9472DDCA6B1B}"/>
+    <workbookView xWindow="3860" yWindow="500" windowWidth="47300" windowHeight="28300" activeTab="2" xr2:uid="{FA1526C8-0ACF-E742-8A11-9472DDCA6B1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -4171,7 +4171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD37D7E-5285-F544-8C65-80F674052271}">
   <dimension ref="A1:G591"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A553" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A337" sqref="A337"/>
     </sheetView>
   </sheetViews>
@@ -45121,8 +45121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB0C0294-0BEE-5241-8492-39D23362D774}">
   <dimension ref="A1:C370"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
+      <selection activeCell="B176" sqref="B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>